<commit_message>
[docs] update system requirement
update system requirement
</commit_message>
<xml_diff>
--- a/docs/01_system_requirement/requirements_v2.0.xlsx
+++ b/docs/01_system_requirement/requirements_v2.0.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\cmu_project\docs\01_system_requirement\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\study\security\cmu\temp\cmu_project\docs\01_system_requirement\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="163">
   <si>
     <t>Requirements from CMU documents on left</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -621,6 +621,31 @@
     <t>considered</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
+  <si>
+    <t>SR-01</t>
+  </si>
+  <si>
+    <t>SR-13</t>
+  </si>
+  <si>
+    <t>SR-03</t>
+  </si>
+  <si>
+    <t>artifacts</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>code review &amp; SA</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SA</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mitigated Art.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -836,7 +861,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -960,6 +985,15 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1017,14 +1051,11 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -19333,8 +19364,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="J2:X42"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="H1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="Q38" sqref="Q38"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="H13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="T34" sqref="T34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -19358,80 +19389,80 @@
   </cols>
   <sheetData>
     <row r="2" spans="10:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="J2" s="44" t="s">
+      <c r="J2" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="K2" s="44"/>
-      <c r="L2" s="44"/>
-      <c r="M2" s="44"/>
-      <c r="O2" s="46" t="s">
+      <c r="K2" s="47"/>
+      <c r="L2" s="47"/>
+      <c r="M2" s="47"/>
+      <c r="O2" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="P2" s="44"/>
-      <c r="Q2" s="44"/>
+      <c r="P2" s="47"/>
+      <c r="Q2" s="47"/>
       <c r="R2" s="22"/>
-      <c r="S2" s="47" t="s">
+      <c r="S2" s="50" t="s">
         <v>144</v>
       </c>
       <c r="T2" s="38"/>
       <c r="U2" s="38"/>
-      <c r="W2" s="47" t="s">
+      <c r="W2" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="X2" s="47"/>
+      <c r="X2" s="50"/>
     </row>
     <row r="3" spans="10:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="J3" s="44"/>
-      <c r="K3" s="44"/>
-      <c r="L3" s="44"/>
-      <c r="M3" s="44"/>
-      <c r="O3" s="44"/>
-      <c r="P3" s="44"/>
-      <c r="Q3" s="44"/>
+      <c r="J3" s="47"/>
+      <c r="K3" s="47"/>
+      <c r="L3" s="47"/>
+      <c r="M3" s="47"/>
+      <c r="O3" s="47"/>
+      <c r="P3" s="47"/>
+      <c r="Q3" s="47"/>
       <c r="R3" s="22"/>
-      <c r="S3" s="47"/>
+      <c r="S3" s="50"/>
       <c r="T3" s="38"/>
       <c r="U3" s="38"/>
-      <c r="W3" s="47"/>
-      <c r="X3" s="47"/>
+      <c r="W3" s="50"/>
+      <c r="X3" s="50"/>
     </row>
     <row r="4" spans="10:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="J4" s="45"/>
-      <c r="K4" s="45"/>
-      <c r="L4" s="45"/>
-      <c r="M4" s="45"/>
-      <c r="O4" s="45"/>
-      <c r="P4" s="45"/>
-      <c r="Q4" s="45"/>
+      <c r="J4" s="48"/>
+      <c r="K4" s="48"/>
+      <c r="L4" s="48"/>
+      <c r="M4" s="48"/>
+      <c r="O4" s="48"/>
+      <c r="P4" s="48"/>
+      <c r="Q4" s="48"/>
       <c r="R4" s="23"/>
-      <c r="S4" s="47"/>
+      <c r="S4" s="50"/>
       <c r="T4" s="38"/>
       <c r="U4" s="38"/>
-      <c r="W4" s="47"/>
-      <c r="X4" s="47"/>
+      <c r="W4" s="50"/>
+      <c r="X4" s="50"/>
     </row>
     <row r="5" spans="10:24" ht="40.5" x14ac:dyDescent="0.3">
-      <c r="J5" s="50" t="s">
+      <c r="J5" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="K5" s="51"/>
-      <c r="L5" s="51"/>
-      <c r="M5" s="52"/>
-      <c r="O5" s="41" t="s">
+      <c r="K5" s="54"/>
+      <c r="L5" s="54"/>
+      <c r="M5" s="55"/>
+      <c r="O5" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="P5" s="41"/>
-      <c r="Q5" s="41"/>
+      <c r="P5" s="44"/>
+      <c r="Q5" s="44"/>
       <c r="R5" s="4"/>
       <c r="S5" s="40" t="s">
         <v>152</v>
       </c>
       <c r="T5" s="39"/>
       <c r="U5" s="39"/>
-      <c r="W5" s="48" t="s">
+      <c r="W5" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="X5" s="48"/>
+      <c r="X5" s="51"/>
     </row>
     <row r="6" spans="10:24" x14ac:dyDescent="0.3">
       <c r="J6" s="29"/>
@@ -19454,7 +19485,7 @@
       <c r="R6" s="24"/>
     </row>
     <row r="7" spans="10:24" ht="54" x14ac:dyDescent="0.3">
-      <c r="J7" s="49"/>
+      <c r="J7" s="52"/>
       <c r="K7" s="30" t="s">
         <v>4</v>
       </c>
@@ -19483,7 +19514,7 @@
       </c>
     </row>
     <row r="8" spans="10:24" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="J8" s="49"/>
+      <c r="J8" s="52"/>
       <c r="K8" s="30" t="s">
         <v>10</v>
       </c>
@@ -19499,7 +19530,7 @@
         <v>135</v>
       </c>
       <c r="R8" s="25"/>
-      <c r="S8" s="60" t="s">
+      <c r="S8" s="42" t="s">
         <v>153</v>
       </c>
       <c r="W8" s="8" t="s">
@@ -19510,7 +19541,7 @@
       </c>
     </row>
     <row r="9" spans="10:24" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="J9" s="49"/>
+      <c r="J9" s="52"/>
       <c r="K9" s="30" t="s">
         <v>15</v>
       </c>
@@ -19537,7 +19568,7 @@
       </c>
     </row>
     <row r="10" spans="10:24" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="J10" s="49"/>
+      <c r="J10" s="52"/>
       <c r="K10" s="30" t="s">
         <v>20</v>
       </c>
@@ -19564,7 +19595,7 @@
       </c>
     </row>
     <row r="11" spans="10:24" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="J11" s="49"/>
+      <c r="J11" s="52"/>
       <c r="K11" s="30" t="s">
         <v>25</v>
       </c>
@@ -19591,7 +19622,7 @@
       </c>
     </row>
     <row r="12" spans="10:24" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="J12" s="49"/>
+      <c r="J12" s="52"/>
       <c r="K12" s="30" t="s">
         <v>30</v>
       </c>
@@ -19618,7 +19649,7 @@
       </c>
     </row>
     <row r="13" spans="10:24" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="J13" s="49"/>
+      <c r="J13" s="52"/>
       <c r="K13" s="30" t="s">
         <v>36</v>
       </c>
@@ -19645,7 +19676,7 @@
       </c>
     </row>
     <row r="14" spans="10:24" x14ac:dyDescent="0.3">
-      <c r="J14" s="49"/>
+      <c r="J14" s="52"/>
       <c r="K14" s="30" t="s">
         <v>41</v>
       </c>
@@ -19659,7 +19690,7 @@
       <c r="R14" s="24"/>
     </row>
     <row r="15" spans="10:24" x14ac:dyDescent="0.3">
-      <c r="J15" s="49"/>
+      <c r="J15" s="52"/>
       <c r="K15" s="30" t="s">
         <v>42</v>
       </c>
@@ -19673,7 +19704,7 @@
       <c r="R15" s="24"/>
     </row>
     <row r="16" spans="10:24" ht="27" x14ac:dyDescent="0.3">
-      <c r="J16" s="49"/>
+      <c r="J16" s="52"/>
       <c r="K16" s="30" t="s">
         <v>43</v>
       </c>
@@ -19689,7 +19720,7 @@
       <c r="R16" s="24"/>
     </row>
     <row r="17" spans="10:24" ht="27" x14ac:dyDescent="0.3">
-      <c r="J17" s="49"/>
+      <c r="J17" s="52"/>
       <c r="K17" s="30" t="s">
         <v>45</v>
       </c>
@@ -19705,7 +19736,7 @@
       <c r="R17" s="24"/>
     </row>
     <row r="18" spans="10:24" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="J18" s="49"/>
+      <c r="J18" s="52"/>
       <c r="K18" s="30" t="s">
         <v>47</v>
       </c>
@@ -19732,7 +19763,7 @@
       </c>
     </row>
     <row r="19" spans="10:24" x14ac:dyDescent="0.3">
-      <c r="J19" s="49"/>
+      <c r="J19" s="52"/>
       <c r="K19" s="30" t="s">
         <v>52</v>
       </c>
@@ -19748,7 +19779,7 @@
       <c r="R19" s="24"/>
     </row>
     <row r="20" spans="10:24" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="J20" s="49"/>
+      <c r="J20" s="52"/>
       <c r="K20" s="30" t="s">
         <v>54</v>
       </c>
@@ -19764,8 +19795,11 @@
         <v>55</v>
       </c>
       <c r="R20" s="24"/>
-      <c r="S20" s="61" t="s">
+      <c r="S20" s="42" t="s">
         <v>153</v>
+      </c>
+      <c r="T20" s="1" t="s">
+        <v>156</v>
       </c>
       <c r="W20" s="8" t="s">
         <v>57</v>
@@ -19775,7 +19809,7 @@
       </c>
     </row>
     <row r="21" spans="10:24" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="J21" s="49"/>
+      <c r="J21" s="52"/>
       <c r="K21" s="30" t="s">
         <v>59</v>
       </c>
@@ -19791,8 +19825,11 @@
         <v>60</v>
       </c>
       <c r="R21" s="24"/>
-      <c r="S21" s="61" t="s">
+      <c r="S21" s="42" t="s">
         <v>153</v>
+      </c>
+      <c r="T21" t="s">
+        <v>157</v>
       </c>
       <c r="W21" s="8" t="s">
         <v>62</v>
@@ -19802,7 +19839,7 @@
       </c>
     </row>
     <row r="22" spans="10:24" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="J22" s="49"/>
+      <c r="J22" s="52"/>
       <c r="K22" s="30" t="s">
         <v>64</v>
       </c>
@@ -19818,7 +19855,7 @@
         <v>65</v>
       </c>
       <c r="R22" s="24"/>
-      <c r="S22" s="60" t="s">
+      <c r="S22" s="41" t="s">
         <v>154</v>
       </c>
       <c r="W22" s="8" t="s">
@@ -19829,7 +19866,7 @@
       </c>
     </row>
     <row r="23" spans="10:24" x14ac:dyDescent="0.3">
-      <c r="J23" s="49"/>
+      <c r="J23" s="52"/>
       <c r="K23" s="30" t="s">
         <v>68</v>
       </c>
@@ -19845,7 +19882,7 @@
       <c r="R23" s="24"/>
     </row>
     <row r="24" spans="10:24" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="J24" s="49"/>
+      <c r="J24" s="52"/>
       <c r="K24" s="30" t="s">
         <v>70</v>
       </c>
@@ -19861,7 +19898,7 @@
         <v>137</v>
       </c>
       <c r="R24" s="24"/>
-      <c r="S24" s="60" t="s">
+      <c r="S24" s="41" t="s">
         <v>154</v>
       </c>
       <c r="W24" s="8" t="s">
@@ -19872,7 +19909,7 @@
       </c>
     </row>
     <row r="25" spans="10:24" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="J25" s="49"/>
+      <c r="J25" s="52"/>
       <c r="K25" s="30" t="s">
         <v>74</v>
       </c>
@@ -19899,7 +19936,7 @@
       </c>
     </row>
     <row r="26" spans="10:24" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="J26" s="49"/>
+      <c r="J26" s="52"/>
       <c r="K26" s="30" t="s">
         <v>79</v>
       </c>
@@ -19915,9 +19952,10 @@
         <v>80</v>
       </c>
       <c r="R26" s="24"/>
-      <c r="S26" s="61" t="s">
+      <c r="S26" s="26" t="s">
         <v>153</v>
       </c>
+      <c r="T26"/>
       <c r="W26" s="8" t="s">
         <v>82</v>
       </c>
@@ -19926,7 +19964,7 @@
       </c>
     </row>
     <row r="27" spans="10:24" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="J27" s="49"/>
+      <c r="J27" s="52"/>
       <c r="K27" s="34" t="s">
         <v>83</v>
       </c>
@@ -19942,10 +19980,12 @@
         <v>84</v>
       </c>
       <c r="R27" s="24"/>
-      <c r="S27" s="62" t="s">
+      <c r="S27" s="43" t="s">
         <v>155</v>
       </c>
-      <c r="T27" s="21"/>
+      <c r="T27" t="s">
+        <v>158</v>
+      </c>
       <c r="U27" s="21"/>
       <c r="V27" s="21"/>
       <c r="W27" s="8" t="s">
@@ -19956,22 +19996,22 @@
       </c>
     </row>
     <row r="28" spans="10:24" ht="14.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="J28" s="41" t="s">
+      <c r="J28" s="44" t="s">
         <v>87</v>
       </c>
-      <c r="K28" s="41"/>
+      <c r="K28" s="44"/>
       <c r="L28" s="27"/>
       <c r="M28" s="28"/>
-      <c r="O28" s="42" t="s">
+      <c r="O28" s="45" t="s">
         <v>87</v>
       </c>
-      <c r="P28" s="42"/>
-      <c r="Q28" s="42"/>
+      <c r="P28" s="45"/>
+      <c r="Q28" s="45"/>
       <c r="R28" s="4"/>
-      <c r="W28" s="43" t="s">
+      <c r="W28" s="46" t="s">
         <v>87</v>
       </c>
-      <c r="X28" s="43"/>
+      <c r="X28" s="46"/>
     </row>
     <row r="29" spans="10:24" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
       <c r="J29" s="30"/>
@@ -19993,6 +20033,9 @@
       <c r="S29" s="1" t="s">
         <v>153</v>
       </c>
+      <c r="T29" s="1" t="s">
+        <v>159</v>
+      </c>
       <c r="W29" s="8" t="s">
         <v>92</v>
       </c>
@@ -20017,8 +20060,11 @@
         <v>95</v>
       </c>
       <c r="R30" s="5"/>
-      <c r="S30" s="60" t="s">
+      <c r="S30" s="42" t="s">
         <v>153</v>
+      </c>
+      <c r="T30" s="1" t="s">
+        <v>160</v>
       </c>
       <c r="W30" s="8" t="s">
         <v>97</v>
@@ -20071,8 +20117,11 @@
         <v>104</v>
       </c>
       <c r="R32" s="5"/>
-      <c r="S32" s="60" t="s">
+      <c r="S32" s="42" t="s">
         <v>153</v>
+      </c>
+      <c r="T32" s="1" t="s">
+        <v>161</v>
       </c>
       <c r="W32" s="8" t="s">
         <v>106</v>
@@ -20101,6 +20150,9 @@
       <c r="S33" s="1" t="s">
         <v>153</v>
       </c>
+      <c r="T33" s="1" t="s">
+        <v>162</v>
+      </c>
       <c r="W33" s="8" t="s">
         <v>111</v>
       </c>
@@ -20147,9 +20199,10 @@
         <v>120</v>
       </c>
       <c r="O35" s="30"/>
-      <c r="P35" s="30"/>
-      <c r="Q35" s="32"/>
+      <c r="P35" s="63"/>
+      <c r="Q35" s="64"/>
       <c r="R35" s="24"/>
+      <c r="S35" s="26"/>
     </row>
     <row r="36" spans="10:24" x14ac:dyDescent="0.3">
       <c r="J36" s="30"/>
@@ -20291,8 +20344,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="J2:X42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="X14" sqref="X14"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -20315,76 +20368,76 @@
   </cols>
   <sheetData>
     <row r="2" spans="10:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="J2" s="56" t="s">
+      <c r="J2" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="K2" s="56"/>
-      <c r="L2" s="56"/>
-      <c r="M2" s="56"/>
-      <c r="O2" s="58" t="s">
+      <c r="K2" s="59"/>
+      <c r="L2" s="59"/>
+      <c r="M2" s="59"/>
+      <c r="O2" s="61" t="s">
         <v>1</v>
       </c>
-      <c r="P2" s="56"/>
-      <c r="Q2" s="56"/>
-      <c r="S2" s="47" t="s">
+      <c r="P2" s="59"/>
+      <c r="Q2" s="59"/>
+      <c r="S2" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="T2" s="47"/>
-      <c r="V2" s="47" t="s">
+      <c r="T2" s="50"/>
+      <c r="V2" s="50" t="s">
         <v>146</v>
       </c>
-      <c r="W2" s="47"/>
-      <c r="X2" s="47"/>
+      <c r="W2" s="50"/>
+      <c r="X2" s="50"/>
     </row>
     <row r="3" spans="10:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="J3" s="56"/>
-      <c r="K3" s="56"/>
-      <c r="L3" s="56"/>
-      <c r="M3" s="56"/>
-      <c r="O3" s="56"/>
-      <c r="P3" s="56"/>
-      <c r="Q3" s="56"/>
-      <c r="S3" s="47"/>
-      <c r="T3" s="47"/>
-      <c r="V3" s="47"/>
-      <c r="W3" s="47"/>
-      <c r="X3" s="47"/>
+      <c r="J3" s="59"/>
+      <c r="K3" s="59"/>
+      <c r="L3" s="59"/>
+      <c r="M3" s="59"/>
+      <c r="O3" s="59"/>
+      <c r="P3" s="59"/>
+      <c r="Q3" s="59"/>
+      <c r="S3" s="50"/>
+      <c r="T3" s="50"/>
+      <c r="V3" s="50"/>
+      <c r="W3" s="50"/>
+      <c r="X3" s="50"/>
     </row>
     <row r="4" spans="10:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="J4" s="57"/>
-      <c r="K4" s="57"/>
-      <c r="L4" s="57"/>
-      <c r="M4" s="57"/>
-      <c r="O4" s="57"/>
-      <c r="P4" s="57"/>
-      <c r="Q4" s="57"/>
-      <c r="S4" s="47"/>
-      <c r="T4" s="47"/>
-      <c r="V4" s="47"/>
-      <c r="W4" s="47"/>
-      <c r="X4" s="47"/>
+      <c r="J4" s="60"/>
+      <c r="K4" s="60"/>
+      <c r="L4" s="60"/>
+      <c r="M4" s="60"/>
+      <c r="O4" s="60"/>
+      <c r="P4" s="60"/>
+      <c r="Q4" s="60"/>
+      <c r="S4" s="50"/>
+      <c r="T4" s="50"/>
+      <c r="V4" s="50"/>
+      <c r="W4" s="50"/>
+      <c r="X4" s="50"/>
     </row>
     <row r="5" spans="10:24" ht="14.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="J5" s="59" t="s">
+      <c r="J5" s="62" t="s">
         <v>3</v>
       </c>
-      <c r="K5" s="59"/>
+      <c r="K5" s="62"/>
       <c r="L5" s="20"/>
       <c r="M5" s="2"/>
-      <c r="O5" s="48" t="s">
+      <c r="O5" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="P5" s="48"/>
-      <c r="Q5" s="48"/>
-      <c r="S5" s="48" t="s">
+      <c r="P5" s="51"/>
+      <c r="Q5" s="51"/>
+      <c r="S5" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="T5" s="48"/>
-      <c r="V5" s="55" t="s">
+      <c r="T5" s="51"/>
+      <c r="V5" s="58" t="s">
         <v>147</v>
       </c>
-      <c r="W5" s="55"/>
-      <c r="X5" s="55"/>
+      <c r="W5" s="58"/>
+      <c r="X5" s="58"/>
     </row>
     <row r="6" spans="10:24" ht="14.25" thickTop="1" x14ac:dyDescent="0.3">
       <c r="J6" s="3"/>
@@ -20395,7 +20448,7 @@
       <c r="Q6" s="6"/>
     </row>
     <row r="7" spans="10:24" ht="54" x14ac:dyDescent="0.3">
-      <c r="J7" s="53"/>
+      <c r="J7" s="56"/>
       <c r="K7" s="1" t="s">
         <v>4</v>
       </c>
@@ -20419,7 +20472,7 @@
       </c>
     </row>
     <row r="8" spans="10:24" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="J8" s="53"/>
+      <c r="J8" s="56"/>
       <c r="K8" s="1" t="s">
         <v>10</v>
       </c>
@@ -20440,7 +20493,7 @@
       </c>
     </row>
     <row r="9" spans="10:24" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="J9" s="53"/>
+      <c r="J9" s="56"/>
       <c r="K9" s="1" t="s">
         <v>15</v>
       </c>
@@ -20461,7 +20514,7 @@
       </c>
     </row>
     <row r="10" spans="10:24" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="J10" s="53"/>
+      <c r="J10" s="56"/>
       <c r="K10" s="1" t="s">
         <v>20</v>
       </c>
@@ -20482,7 +20535,7 @@
       </c>
     </row>
     <row r="11" spans="10:24" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="J11" s="53"/>
+      <c r="J11" s="56"/>
       <c r="K11" s="1" t="s">
         <v>25</v>
       </c>
@@ -20503,7 +20556,7 @@
       </c>
     </row>
     <row r="12" spans="10:24" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="J12" s="53"/>
+      <c r="J12" s="56"/>
       <c r="K12" s="1" t="s">
         <v>30</v>
       </c>
@@ -20524,7 +20577,7 @@
       </c>
     </row>
     <row r="13" spans="10:24" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="J13" s="53"/>
+      <c r="J13" s="56"/>
       <c r="K13" s="1" t="s">
         <v>36</v>
       </c>
@@ -20545,7 +20598,7 @@
       </c>
     </row>
     <row r="14" spans="10:24" x14ac:dyDescent="0.3">
-      <c r="J14" s="53"/>
+      <c r="J14" s="56"/>
       <c r="K14" s="1" t="s">
         <v>41</v>
       </c>
@@ -20555,7 +20608,7 @@
       <c r="Q14" s="6"/>
     </row>
     <row r="15" spans="10:24" x14ac:dyDescent="0.3">
-      <c r="J15" s="53"/>
+      <c r="J15" s="56"/>
       <c r="K15" s="1" t="s">
         <v>42</v>
       </c>
@@ -20565,7 +20618,7 @@
       <c r="Q15" s="6"/>
     </row>
     <row r="16" spans="10:24" ht="27" x14ac:dyDescent="0.3">
-      <c r="J16" s="53"/>
+      <c r="J16" s="56"/>
       <c r="K16" s="1" t="s">
         <v>43</v>
       </c>
@@ -20579,7 +20632,7 @@
       <c r="Q16" s="6"/>
     </row>
     <row r="17" spans="10:24" ht="27" x14ac:dyDescent="0.3">
-      <c r="J17" s="53"/>
+      <c r="J17" s="56"/>
       <c r="K17" s="1" t="s">
         <v>45</v>
       </c>
@@ -20593,7 +20646,7 @@
       <c r="Q17" s="6"/>
     </row>
     <row r="18" spans="10:24" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="J18" s="53"/>
+      <c r="J18" s="56"/>
       <c r="K18" s="1" t="s">
         <v>47</v>
       </c>
@@ -20617,7 +20670,7 @@
       </c>
     </row>
     <row r="19" spans="10:24" x14ac:dyDescent="0.3">
-      <c r="J19" s="53"/>
+      <c r="J19" s="56"/>
       <c r="K19" s="1" t="s">
         <v>52</v>
       </c>
@@ -20630,7 +20683,7 @@
       <c r="Q19" s="6"/>
     </row>
     <row r="20" spans="10:24" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="J20" s="53"/>
+      <c r="J20" s="56"/>
       <c r="K20" s="1" t="s">
         <v>54</v>
       </c>
@@ -20651,7 +20704,7 @@
       </c>
     </row>
     <row r="21" spans="10:24" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="J21" s="53"/>
+      <c r="J21" s="56"/>
       <c r="K21" s="1" t="s">
         <v>59</v>
       </c>
@@ -20672,7 +20725,7 @@
       </c>
     </row>
     <row r="22" spans="10:24" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="J22" s="53"/>
+      <c r="J22" s="56"/>
       <c r="K22" s="1" t="s">
         <v>64</v>
       </c>
@@ -20696,7 +20749,7 @@
       </c>
     </row>
     <row r="23" spans="10:24" x14ac:dyDescent="0.3">
-      <c r="J23" s="53"/>
+      <c r="J23" s="56"/>
       <c r="K23" s="1" t="s">
         <v>68</v>
       </c>
@@ -20709,7 +20762,7 @@
       <c r="Q23" s="6"/>
     </row>
     <row r="24" spans="10:24" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="J24" s="53"/>
+      <c r="J24" s="56"/>
       <c r="K24" s="1" t="s">
         <v>70</v>
       </c>
@@ -20733,7 +20786,7 @@
       </c>
     </row>
     <row r="25" spans="10:24" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="J25" s="53"/>
+      <c r="J25" s="56"/>
       <c r="K25" s="1" t="s">
         <v>74</v>
       </c>
@@ -20757,7 +20810,7 @@
       </c>
     </row>
     <row r="26" spans="10:24" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="J26" s="53"/>
+      <c r="J26" s="56"/>
       <c r="K26" s="1" t="s">
         <v>79</v>
       </c>
@@ -20778,7 +20831,7 @@
       </c>
     </row>
     <row r="27" spans="10:24" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="J27" s="53"/>
+      <c r="J27" s="56"/>
       <c r="K27" s="10" t="s">
         <v>83</v>
       </c>
@@ -20805,21 +20858,21 @@
       <c r="X27" s="21"/>
     </row>
     <row r="28" spans="10:24" ht="14.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="J28" s="54" t="s">
+      <c r="J28" s="57" t="s">
         <v>87</v>
       </c>
-      <c r="K28" s="54"/>
+      <c r="K28" s="57"/>
       <c r="L28" s="19"/>
       <c r="M28" s="11"/>
-      <c r="O28" s="43" t="s">
+      <c r="O28" s="46" t="s">
         <v>87</v>
       </c>
-      <c r="P28" s="43"/>
-      <c r="Q28" s="43"/>
-      <c r="S28" s="43" t="s">
+      <c r="P28" s="46"/>
+      <c r="Q28" s="46"/>
+      <c r="S28" s="46" t="s">
         <v>87</v>
       </c>
-      <c r="T28" s="43"/>
+      <c r="T28" s="46"/>
     </row>
     <row r="29" spans="10:24" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
       <c r="K29" s="12" t="s">

</xml_diff>

<commit_message>
[docs] update phase1 document
update pahse1 document
</commit_message>
<xml_diff>
--- a/docs/01_system_requirement/requirements_v2.0.xlsx
+++ b/docs/01_system_requirement/requirements_v2.0.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\cmu_project\docs\01_system_requirement\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\study\security\cmu\temp\cmu_project\docs\01_system_requirement\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="175">
   <si>
     <t>Requirements from CMU documents on left</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -672,6 +672,30 @@
     <t>SR-09</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
+  <si>
+    <t>CMU-REQ-D-02</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>CMU-REQ-D-10</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>CMU-REQ-D-15</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>구현여부</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>O</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Implement</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -1005,9 +1029,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1022,6 +1043,21 @@
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1039,6 +1075,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1080,22 +1119,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -19406,7 +19430,7 @@
   <dimension ref="J2:X42"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Q38" sqref="Q38"/>
+      <selection activeCell="U40" sqref="U40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -19423,88 +19447,93 @@
     <col min="17" max="17" width="46.625" style="1" customWidth="1"/>
     <col min="18" max="18" width="13.5" style="26" hidden="1" customWidth="1"/>
     <col min="19" max="19" width="14.875" style="1" customWidth="1"/>
-    <col min="20" max="22" width="13.5" style="1" customWidth="1"/>
+    <col min="20" max="20" width="16.5" style="1" customWidth="1"/>
+    <col min="21" max="22" width="13.5" style="1" customWidth="1"/>
     <col min="23" max="23" width="12.5" style="1" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="56.25" style="1" customWidth="1"/>
     <col min="25" max="16384" width="8.625" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="10:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="J2" s="48" t="s">
+      <c r="J2" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="K2" s="48"/>
-      <c r="L2" s="48"/>
-      <c r="M2" s="48"/>
-      <c r="O2" s="50" t="s">
+      <c r="K2" s="52"/>
+      <c r="L2" s="52"/>
+      <c r="M2" s="52"/>
+      <c r="O2" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="P2" s="48"/>
-      <c r="Q2" s="48"/>
+      <c r="P2" s="52"/>
+      <c r="Q2" s="52"/>
       <c r="R2" s="22"/>
-      <c r="S2" s="51" t="s">
+      <c r="S2" s="56" t="s">
         <v>144</v>
       </c>
       <c r="T2" s="38"/>
       <c r="U2" s="38"/>
-      <c r="W2" s="64" t="s">
+      <c r="W2" s="55" t="s">
         <v>161</v>
       </c>
-      <c r="X2" s="51"/>
+      <c r="X2" s="56"/>
     </row>
     <row r="3" spans="10:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="J3" s="48"/>
-      <c r="K3" s="48"/>
-      <c r="L3" s="48"/>
-      <c r="M3" s="48"/>
-      <c r="O3" s="48"/>
-      <c r="P3" s="48"/>
-      <c r="Q3" s="48"/>
+      <c r="J3" s="52"/>
+      <c r="K3" s="52"/>
+      <c r="L3" s="52"/>
+      <c r="M3" s="52"/>
+      <c r="O3" s="52"/>
+      <c r="P3" s="52"/>
+      <c r="Q3" s="52"/>
       <c r="R3" s="22"/>
-      <c r="S3" s="51"/>
-      <c r="U3" s="38"/>
-      <c r="W3" s="51"/>
-      <c r="X3" s="51"/>
+      <c r="S3" s="56"/>
+      <c r="U3" s="38" t="s">
+        <v>174</v>
+      </c>
+      <c r="W3" s="56"/>
+      <c r="X3" s="56"/>
     </row>
     <row r="4" spans="10:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="J4" s="49"/>
-      <c r="K4" s="49"/>
-      <c r="L4" s="49"/>
-      <c r="M4" s="49"/>
-      <c r="O4" s="49"/>
-      <c r="P4" s="49"/>
-      <c r="Q4" s="49"/>
+      <c r="J4" s="53"/>
+      <c r="K4" s="53"/>
+      <c r="L4" s="53"/>
+      <c r="M4" s="53"/>
+      <c r="O4" s="53"/>
+      <c r="P4" s="53"/>
+      <c r="Q4" s="53"/>
       <c r="R4" s="23"/>
-      <c r="S4" s="51"/>
+      <c r="S4" s="56"/>
       <c r="T4" s="38"/>
       <c r="U4" s="38"/>
-      <c r="W4" s="51"/>
-      <c r="X4" s="51"/>
+      <c r="W4" s="56"/>
+      <c r="X4" s="56"/>
     </row>
     <row r="5" spans="10:24" ht="54" x14ac:dyDescent="0.3">
-      <c r="J5" s="54" t="s">
+      <c r="J5" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="K5" s="55"/>
-      <c r="L5" s="55"/>
-      <c r="M5" s="56"/>
-      <c r="O5" s="45" t="s">
+      <c r="K5" s="60"/>
+      <c r="L5" s="60"/>
+      <c r="M5" s="61"/>
+      <c r="O5" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="P5" s="45"/>
-      <c r="Q5" s="45"/>
+      <c r="P5" s="49"/>
+      <c r="Q5" s="49"/>
       <c r="R5" s="4"/>
-      <c r="S5" s="40" t="s">
+      <c r="S5" s="39" t="s">
         <v>163</v>
       </c>
-      <c r="T5" s="69" t="s">
+      <c r="T5" s="48" t="s">
         <v>162</v>
       </c>
-      <c r="U5" s="39"/>
-      <c r="W5" s="52" t="s">
+      <c r="U5" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="W5" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="X5" s="52"/>
+      <c r="X5" s="57"/>
     </row>
     <row r="6" spans="10:24" x14ac:dyDescent="0.3">
       <c r="J6" s="29"/>
@@ -19525,10 +19554,10 @@
         <v>151</v>
       </c>
       <c r="R6" s="24"/>
-      <c r="T6" s="42"/>
+      <c r="T6" s="41"/>
     </row>
     <row r="7" spans="10:24" ht="54" x14ac:dyDescent="0.3">
-      <c r="J7" s="53"/>
+      <c r="J7" s="58"/>
       <c r="K7" s="30" t="s">
         <v>4</v>
       </c>
@@ -19549,7 +19578,10 @@
       <c r="S7" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="T7" s="42"/>
+      <c r="T7" s="41"/>
+      <c r="U7" s="69" t="s">
+        <v>173</v>
+      </c>
       <c r="W7" s="8" t="s">
         <v>8</v>
       </c>
@@ -19558,7 +19590,7 @@
       </c>
     </row>
     <row r="8" spans="10:24" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="J8" s="53"/>
+      <c r="J8" s="58"/>
       <c r="K8" s="30" t="s">
         <v>10</v>
       </c>
@@ -19568,17 +19600,20 @@
       </c>
       <c r="O8" s="30"/>
       <c r="P8" s="36" t="s">
-        <v>12</v>
+        <v>169</v>
       </c>
       <c r="Q8" s="33" t="s">
         <v>135</v>
       </c>
       <c r="R8" s="25"/>
-      <c r="S8" s="41" t="s">
+      <c r="S8" s="40" t="s">
         <v>167</v>
       </c>
-      <c r="T8" s="42" t="s">
+      <c r="T8" s="41" t="s">
         <v>168</v>
+      </c>
+      <c r="U8" s="1" t="s">
+        <v>173</v>
       </c>
       <c r="W8" s="8" t="s">
         <v>13</v>
@@ -19588,7 +19623,7 @@
       </c>
     </row>
     <row r="9" spans="10:24" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="J9" s="53"/>
+      <c r="J9" s="58"/>
       <c r="K9" s="30" t="s">
         <v>15</v>
       </c>
@@ -19607,7 +19642,10 @@
       <c r="S9" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="T9" s="42"/>
+      <c r="T9" s="41"/>
+      <c r="U9" s="1" t="s">
+        <v>173</v>
+      </c>
       <c r="W9" s="8" t="s">
         <v>18</v>
       </c>
@@ -19616,7 +19654,7 @@
       </c>
     </row>
     <row r="10" spans="10:24" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="J10" s="53"/>
+      <c r="J10" s="58"/>
       <c r="K10" s="30" t="s">
         <v>20</v>
       </c>
@@ -19635,7 +19673,10 @@
       <c r="S10" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="T10" s="42"/>
+      <c r="T10" s="41"/>
+      <c r="U10" s="1" t="s">
+        <v>173</v>
+      </c>
       <c r="W10" s="8" t="s">
         <v>23</v>
       </c>
@@ -19644,7 +19685,7 @@
       </c>
     </row>
     <row r="11" spans="10:24" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="J11" s="53"/>
+      <c r="J11" s="58"/>
       <c r="K11" s="30" t="s">
         <v>25</v>
       </c>
@@ -19663,7 +19704,10 @@
       <c r="S11" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="T11" s="42"/>
+      <c r="T11" s="41"/>
+      <c r="U11" s="1" t="s">
+        <v>173</v>
+      </c>
       <c r="W11" s="8" t="s">
         <v>28</v>
       </c>
@@ -19672,7 +19716,7 @@
       </c>
     </row>
     <row r="12" spans="10:24" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="J12" s="53"/>
+      <c r="J12" s="58"/>
       <c r="K12" s="30" t="s">
         <v>30</v>
       </c>
@@ -19691,7 +19735,10 @@
       <c r="S12" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="T12" s="42"/>
+      <c r="T12" s="41"/>
+      <c r="U12" s="1" t="s">
+        <v>173</v>
+      </c>
       <c r="W12" s="8" t="s">
         <v>34</v>
       </c>
@@ -19700,7 +19747,7 @@
       </c>
     </row>
     <row r="13" spans="10:24" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="J13" s="53"/>
+      <c r="J13" s="58"/>
       <c r="K13" s="30" t="s">
         <v>36</v>
       </c>
@@ -19719,7 +19766,10 @@
       <c r="S13" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="T13" s="42"/>
+      <c r="T13" s="41"/>
+      <c r="U13" s="1" t="s">
+        <v>173</v>
+      </c>
       <c r="W13" s="8" t="s">
         <v>39</v>
       </c>
@@ -19728,7 +19778,7 @@
       </c>
     </row>
     <row r="14" spans="10:24" hidden="1" x14ac:dyDescent="0.3">
-      <c r="J14" s="53"/>
+      <c r="J14" s="58"/>
       <c r="K14" s="30" t="s">
         <v>41</v>
       </c>
@@ -19740,10 +19790,10 @@
       <c r="P14" s="30"/>
       <c r="Q14" s="32"/>
       <c r="R14" s="24"/>
-      <c r="T14" s="42"/>
+      <c r="T14" s="41"/>
     </row>
     <row r="15" spans="10:24" hidden="1" x14ac:dyDescent="0.3">
-      <c r="J15" s="53"/>
+      <c r="J15" s="58"/>
       <c r="K15" s="30" t="s">
         <v>42</v>
       </c>
@@ -19755,10 +19805,10 @@
       <c r="P15" s="30"/>
       <c r="Q15" s="32"/>
       <c r="R15" s="24"/>
-      <c r="T15" s="42"/>
+      <c r="T15" s="41"/>
     </row>
     <row r="16" spans="10:24" ht="27" hidden="1" x14ac:dyDescent="0.3">
-      <c r="J16" s="53"/>
+      <c r="J16" s="58"/>
       <c r="K16" s="30" t="s">
         <v>43</v>
       </c>
@@ -19772,10 +19822,10 @@
       <c r="P16" s="31"/>
       <c r="Q16" s="32"/>
       <c r="R16" s="24"/>
-      <c r="T16" s="42"/>
+      <c r="T16" s="41"/>
     </row>
     <row r="17" spans="10:24" ht="27" hidden="1" x14ac:dyDescent="0.3">
-      <c r="J17" s="53"/>
+      <c r="J17" s="58"/>
       <c r="K17" s="30" t="s">
         <v>45</v>
       </c>
@@ -19789,10 +19839,10 @@
       <c r="P17" s="31"/>
       <c r="Q17" s="32"/>
       <c r="R17" s="24"/>
-      <c r="T17" s="42"/>
+      <c r="T17" s="41"/>
     </row>
     <row r="18" spans="10:24" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="J18" s="53"/>
+      <c r="J18" s="58"/>
       <c r="K18" s="30" t="s">
         <v>47</v>
       </c>
@@ -19808,10 +19858,10 @@
         <v>139</v>
       </c>
       <c r="R18" s="24"/>
-      <c r="S18" s="65" t="s">
+      <c r="S18" s="44" t="s">
         <v>152</v>
       </c>
-      <c r="T18" s="42"/>
+      <c r="T18" s="41"/>
       <c r="W18" s="8" t="s">
         <v>50</v>
       </c>
@@ -19820,7 +19870,7 @@
       </c>
     </row>
     <row r="19" spans="10:24" hidden="1" x14ac:dyDescent="0.3">
-      <c r="J19" s="53"/>
+      <c r="J19" s="58"/>
       <c r="K19" s="30" t="s">
         <v>52</v>
       </c>
@@ -19834,10 +19884,10 @@
       <c r="P19" s="30"/>
       <c r="Q19" s="32"/>
       <c r="R19" s="24"/>
-      <c r="T19" s="42"/>
+      <c r="T19" s="41"/>
     </row>
     <row r="20" spans="10:24" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="J20" s="53"/>
+      <c r="J20" s="58"/>
       <c r="K20" s="30" t="s">
         <v>54</v>
       </c>
@@ -19853,11 +19903,14 @@
         <v>55</v>
       </c>
       <c r="R20" s="24"/>
-      <c r="S20" s="41" t="s">
+      <c r="S20" s="40" t="s">
         <v>167</v>
       </c>
-      <c r="T20" s="42" t="s">
+      <c r="T20" s="41" t="s">
         <v>154</v>
+      </c>
+      <c r="U20" s="1" t="s">
+        <v>173</v>
       </c>
       <c r="W20" s="8" t="s">
         <v>57</v>
@@ -19867,7 +19920,7 @@
       </c>
     </row>
     <row r="21" spans="10:24" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="J21" s="53"/>
+      <c r="J21" s="58"/>
       <c r="K21" s="30" t="s">
         <v>59</v>
       </c>
@@ -19877,17 +19930,20 @@
       </c>
       <c r="O21" s="30"/>
       <c r="P21" s="30" t="s">
-        <v>61</v>
+        <v>170</v>
       </c>
       <c r="Q21" s="32" t="s">
         <v>60</v>
       </c>
       <c r="R21" s="24"/>
-      <c r="S21" s="41" t="s">
+      <c r="S21" s="40" t="s">
         <v>167</v>
       </c>
-      <c r="T21" s="67" t="s">
+      <c r="T21" s="46" t="s">
         <v>155</v>
+      </c>
+      <c r="U21" s="1" t="s">
+        <v>173</v>
       </c>
       <c r="W21" s="8" t="s">
         <v>62</v>
@@ -19897,7 +19953,7 @@
       </c>
     </row>
     <row r="22" spans="10:24" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="J22" s="53"/>
+      <c r="J22" s="58"/>
       <c r="K22" s="30" t="s">
         <v>64</v>
       </c>
@@ -19913,10 +19969,10 @@
         <v>65</v>
       </c>
       <c r="R22" s="24"/>
-      <c r="S22" s="65" t="s">
+      <c r="S22" s="44" t="s">
         <v>152</v>
       </c>
-      <c r="T22" s="42"/>
+      <c r="T22" s="41"/>
       <c r="W22" s="8" t="s">
         <v>67</v>
       </c>
@@ -19925,7 +19981,7 @@
       </c>
     </row>
     <row r="23" spans="10:24" hidden="1" x14ac:dyDescent="0.3">
-      <c r="J23" s="53"/>
+      <c r="J23" s="58"/>
       <c r="K23" s="30" t="s">
         <v>68</v>
       </c>
@@ -19939,10 +19995,10 @@
       <c r="P23" s="30"/>
       <c r="Q23" s="32"/>
       <c r="R23" s="24"/>
-      <c r="T23" s="42"/>
+      <c r="T23" s="41"/>
     </row>
     <row r="24" spans="10:24" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="J24" s="53"/>
+      <c r="J24" s="58"/>
       <c r="K24" s="30" t="s">
         <v>70</v>
       </c>
@@ -19958,10 +20014,10 @@
         <v>137</v>
       </c>
       <c r="R24" s="24"/>
-      <c r="S24" s="65" t="s">
+      <c r="S24" s="44" t="s">
         <v>152</v>
       </c>
-      <c r="T24" s="42"/>
+      <c r="T24" s="41"/>
       <c r="W24" s="8" t="s">
         <v>73</v>
       </c>
@@ -19970,7 +20026,7 @@
       </c>
     </row>
     <row r="25" spans="10:24" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="J25" s="53"/>
+      <c r="J25" s="58"/>
       <c r="K25" s="30" t="s">
         <v>74</v>
       </c>
@@ -19989,7 +20045,7 @@
       <c r="S25" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="T25" s="42"/>
+      <c r="T25" s="41"/>
       <c r="W25" s="8" t="s">
         <v>77</v>
       </c>
@@ -19998,7 +20054,7 @@
       </c>
     </row>
     <row r="26" spans="10:24" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="J26" s="53"/>
+      <c r="J26" s="58"/>
       <c r="K26" s="30" t="s">
         <v>79</v>
       </c>
@@ -20017,7 +20073,10 @@
       <c r="S26" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="T26" s="67"/>
+      <c r="T26" s="46"/>
+      <c r="U26" s="1" t="s">
+        <v>173</v>
+      </c>
       <c r="W26" s="8" t="s">
         <v>82</v>
       </c>
@@ -20026,7 +20085,7 @@
       </c>
     </row>
     <row r="27" spans="10:24" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="J27" s="53"/>
+      <c r="J27" s="58"/>
       <c r="K27" s="34" t="s">
         <v>83</v>
       </c>
@@ -20036,19 +20095,21 @@
       </c>
       <c r="O27" s="30"/>
       <c r="P27" s="30" t="s">
-        <v>85</v>
+        <v>171</v>
       </c>
       <c r="Q27" s="32" t="s">
         <v>84</v>
       </c>
       <c r="R27" s="24"/>
-      <c r="S27" s="66" t="s">
+      <c r="S27" s="45" t="s">
         <v>153</v>
       </c>
-      <c r="T27" s="67" t="s">
+      <c r="T27" s="46" t="s">
         <v>156</v>
       </c>
-      <c r="U27" s="21"/>
+      <c r="U27" s="1" t="s">
+        <v>173</v>
+      </c>
       <c r="V27" s="21"/>
       <c r="W27" s="8" t="s">
         <v>86</v>
@@ -20058,23 +20119,23 @@
       </c>
     </row>
     <row r="28" spans="10:24" ht="14.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="J28" s="45" t="s">
+      <c r="J28" s="49" t="s">
         <v>87</v>
       </c>
-      <c r="K28" s="45"/>
+      <c r="K28" s="49"/>
       <c r="L28" s="27"/>
       <c r="M28" s="28"/>
-      <c r="O28" s="46" t="s">
+      <c r="O28" s="50" t="s">
         <v>87</v>
       </c>
-      <c r="P28" s="46"/>
-      <c r="Q28" s="46"/>
+      <c r="P28" s="50"/>
+      <c r="Q28" s="50"/>
       <c r="R28" s="4"/>
-      <c r="T28" s="42"/>
-      <c r="W28" s="47" t="s">
+      <c r="T28" s="41"/>
+      <c r="W28" s="51" t="s">
         <v>87</v>
       </c>
-      <c r="X28" s="47"/>
+      <c r="X28" s="51"/>
     </row>
     <row r="29" spans="10:24" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
       <c r="J29" s="30"/>
@@ -20096,8 +20157,11 @@
       <c r="S29" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="T29" s="42" t="s">
+      <c r="T29" s="41" t="s">
         <v>158</v>
+      </c>
+      <c r="U29" s="1" t="s">
+        <v>173</v>
       </c>
       <c r="W29" s="8" t="s">
         <v>92</v>
@@ -20123,11 +20187,14 @@
         <v>95</v>
       </c>
       <c r="R30" s="5"/>
-      <c r="S30" s="41" t="s">
+      <c r="S30" s="40" t="s">
         <v>166</v>
       </c>
-      <c r="T30" s="68" t="s">
+      <c r="T30" s="47" t="s">
         <v>159</v>
+      </c>
+      <c r="U30" s="1" t="s">
+        <v>173</v>
       </c>
       <c r="W30" s="8" t="s">
         <v>97</v>
@@ -20156,7 +20223,10 @@
       <c r="S31" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="T31" s="42"/>
+      <c r="T31" s="41"/>
+      <c r="U31" s="1" t="s">
+        <v>173</v>
+      </c>
       <c r="W31" s="8" t="s">
         <v>101</v>
       </c>
@@ -20181,11 +20251,14 @@
         <v>104</v>
       </c>
       <c r="R32" s="5"/>
-      <c r="S32" s="41" t="s">
+      <c r="S32" s="40" t="s">
         <v>166</v>
       </c>
-      <c r="T32" s="42" t="s">
+      <c r="T32" s="41" t="s">
         <v>160</v>
+      </c>
+      <c r="U32" s="1" t="s">
+        <v>173</v>
       </c>
       <c r="W32" s="8" t="s">
         <v>106</v>
@@ -20214,8 +20287,11 @@
       <c r="S33" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="T33" s="42" t="s">
+      <c r="T33" s="41" t="s">
         <v>157</v>
+      </c>
+      <c r="U33" s="1" t="s">
+        <v>173</v>
       </c>
       <c r="W33" s="8" t="s">
         <v>111</v>
@@ -20241,7 +20317,7 @@
         <v>114</v>
       </c>
       <c r="R34" s="5"/>
-      <c r="S34" s="65" t="s">
+      <c r="S34" s="44" t="s">
         <v>152</v>
       </c>
       <c r="W34" s="8" t="s">
@@ -20263,8 +20339,8 @@
         <v>120</v>
       </c>
       <c r="O35" s="30"/>
-      <c r="P35" s="43"/>
-      <c r="Q35" s="44"/>
+      <c r="P35" s="42"/>
+      <c r="Q35" s="43"/>
       <c r="R35" s="24"/>
       <c r="S35" s="26"/>
     </row>
@@ -20301,7 +20377,7 @@
         <v>124</v>
       </c>
       <c r="R37" s="5"/>
-      <c r="S37" s="65" t="s">
+      <c r="S37" s="44" t="s">
         <v>152</v>
       </c>
       <c r="W37" s="8" t="s">
@@ -20328,7 +20404,7 @@
         <v>128</v>
       </c>
       <c r="R38" s="5"/>
-      <c r="S38" s="65" t="s">
+      <c r="S38" s="44" t="s">
         <v>152</v>
       </c>
       <c r="W38" s="8" t="s">
@@ -20355,7 +20431,7 @@
         <v>132</v>
       </c>
       <c r="R39" s="5"/>
-      <c r="S39" s="65" t="s">
+      <c r="S39" s="44" t="s">
         <v>152</v>
       </c>
       <c r="W39" s="8" t="s">
@@ -20432,76 +20508,76 @@
   </cols>
   <sheetData>
     <row r="2" spans="10:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="J2" s="60" t="s">
+      <c r="J2" s="65" t="s">
         <v>0</v>
       </c>
-      <c r="K2" s="60"/>
-      <c r="L2" s="60"/>
-      <c r="M2" s="60"/>
-      <c r="O2" s="62" t="s">
+      <c r="K2" s="65"/>
+      <c r="L2" s="65"/>
+      <c r="M2" s="65"/>
+      <c r="O2" s="67" t="s">
         <v>1</v>
       </c>
-      <c r="P2" s="60"/>
-      <c r="Q2" s="60"/>
-      <c r="S2" s="51" t="s">
+      <c r="P2" s="65"/>
+      <c r="Q2" s="65"/>
+      <c r="S2" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="T2" s="51"/>
-      <c r="V2" s="51" t="s">
+      <c r="T2" s="56"/>
+      <c r="V2" s="56" t="s">
         <v>146</v>
       </c>
-      <c r="W2" s="51"/>
-      <c r="X2" s="51"/>
+      <c r="W2" s="56"/>
+      <c r="X2" s="56"/>
     </row>
     <row r="3" spans="10:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="J3" s="60"/>
-      <c r="K3" s="60"/>
-      <c r="L3" s="60"/>
-      <c r="M3" s="60"/>
-      <c r="O3" s="60"/>
-      <c r="P3" s="60"/>
-      <c r="Q3" s="60"/>
-      <c r="S3" s="51"/>
-      <c r="T3" s="51"/>
-      <c r="V3" s="51"/>
-      <c r="W3" s="51"/>
-      <c r="X3" s="51"/>
+      <c r="J3" s="65"/>
+      <c r="K3" s="65"/>
+      <c r="L3" s="65"/>
+      <c r="M3" s="65"/>
+      <c r="O3" s="65"/>
+      <c r="P3" s="65"/>
+      <c r="Q3" s="65"/>
+      <c r="S3" s="56"/>
+      <c r="T3" s="56"/>
+      <c r="V3" s="56"/>
+      <c r="W3" s="56"/>
+      <c r="X3" s="56"/>
     </row>
     <row r="4" spans="10:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="J4" s="61"/>
-      <c r="K4" s="61"/>
-      <c r="L4" s="61"/>
-      <c r="M4" s="61"/>
-      <c r="O4" s="61"/>
-      <c r="P4" s="61"/>
-      <c r="Q4" s="61"/>
-      <c r="S4" s="51"/>
-      <c r="T4" s="51"/>
-      <c r="V4" s="51"/>
-      <c r="W4" s="51"/>
-      <c r="X4" s="51"/>
+      <c r="J4" s="66"/>
+      <c r="K4" s="66"/>
+      <c r="L4" s="66"/>
+      <c r="M4" s="66"/>
+      <c r="O4" s="66"/>
+      <c r="P4" s="66"/>
+      <c r="Q4" s="66"/>
+      <c r="S4" s="56"/>
+      <c r="T4" s="56"/>
+      <c r="V4" s="56"/>
+      <c r="W4" s="56"/>
+      <c r="X4" s="56"/>
     </row>
     <row r="5" spans="10:24" ht="14.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="J5" s="63" t="s">
+      <c r="J5" s="68" t="s">
         <v>3</v>
       </c>
-      <c r="K5" s="63"/>
+      <c r="K5" s="68"/>
       <c r="L5" s="20"/>
       <c r="M5" s="2"/>
-      <c r="O5" s="52" t="s">
+      <c r="O5" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="P5" s="52"/>
-      <c r="Q5" s="52"/>
-      <c r="S5" s="52" t="s">
+      <c r="P5" s="57"/>
+      <c r="Q5" s="57"/>
+      <c r="S5" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="T5" s="52"/>
-      <c r="V5" s="59" t="s">
+      <c r="T5" s="57"/>
+      <c r="V5" s="64" t="s">
         <v>147</v>
       </c>
-      <c r="W5" s="59"/>
-      <c r="X5" s="59"/>
+      <c r="W5" s="64"/>
+      <c r="X5" s="64"/>
     </row>
     <row r="6" spans="10:24" ht="14.25" thickTop="1" x14ac:dyDescent="0.3">
       <c r="J6" s="3"/>
@@ -20512,7 +20588,7 @@
       <c r="Q6" s="6"/>
     </row>
     <row r="7" spans="10:24" ht="54" x14ac:dyDescent="0.3">
-      <c r="J7" s="57"/>
+      <c r="J7" s="62"/>
       <c r="K7" s="1" t="s">
         <v>4</v>
       </c>
@@ -20536,7 +20612,7 @@
       </c>
     </row>
     <row r="8" spans="10:24" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="J8" s="57"/>
+      <c r="J8" s="62"/>
       <c r="K8" s="1" t="s">
         <v>10</v>
       </c>
@@ -20557,7 +20633,7 @@
       </c>
     </row>
     <row r="9" spans="10:24" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="J9" s="57"/>
+      <c r="J9" s="62"/>
       <c r="K9" s="1" t="s">
         <v>15</v>
       </c>
@@ -20578,7 +20654,7 @@
       </c>
     </row>
     <row r="10" spans="10:24" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="J10" s="57"/>
+      <c r="J10" s="62"/>
       <c r="K10" s="1" t="s">
         <v>20</v>
       </c>
@@ -20599,7 +20675,7 @@
       </c>
     </row>
     <row r="11" spans="10:24" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="J11" s="57"/>
+      <c r="J11" s="62"/>
       <c r="K11" s="1" t="s">
         <v>25</v>
       </c>
@@ -20620,7 +20696,7 @@
       </c>
     </row>
     <row r="12" spans="10:24" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="J12" s="57"/>
+      <c r="J12" s="62"/>
       <c r="K12" s="1" t="s">
         <v>30</v>
       </c>
@@ -20641,7 +20717,7 @@
       </c>
     </row>
     <row r="13" spans="10:24" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="J13" s="57"/>
+      <c r="J13" s="62"/>
       <c r="K13" s="1" t="s">
         <v>36</v>
       </c>
@@ -20662,7 +20738,7 @@
       </c>
     </row>
     <row r="14" spans="10:24" x14ac:dyDescent="0.3">
-      <c r="J14" s="57"/>
+      <c r="J14" s="62"/>
       <c r="K14" s="1" t="s">
         <v>41</v>
       </c>
@@ -20672,7 +20748,7 @@
       <c r="Q14" s="6"/>
     </row>
     <row r="15" spans="10:24" x14ac:dyDescent="0.3">
-      <c r="J15" s="57"/>
+      <c r="J15" s="62"/>
       <c r="K15" s="1" t="s">
         <v>42</v>
       </c>
@@ -20682,7 +20758,7 @@
       <c r="Q15" s="6"/>
     </row>
     <row r="16" spans="10:24" ht="27" x14ac:dyDescent="0.3">
-      <c r="J16" s="57"/>
+      <c r="J16" s="62"/>
       <c r="K16" s="1" t="s">
         <v>43</v>
       </c>
@@ -20696,7 +20772,7 @@
       <c r="Q16" s="6"/>
     </row>
     <row r="17" spans="10:24" ht="27" x14ac:dyDescent="0.3">
-      <c r="J17" s="57"/>
+      <c r="J17" s="62"/>
       <c r="K17" s="1" t="s">
         <v>45</v>
       </c>
@@ -20710,7 +20786,7 @@
       <c r="Q17" s="6"/>
     </row>
     <row r="18" spans="10:24" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="J18" s="57"/>
+      <c r="J18" s="62"/>
       <c r="K18" s="1" t="s">
         <v>47</v>
       </c>
@@ -20734,7 +20810,7 @@
       </c>
     </row>
     <row r="19" spans="10:24" x14ac:dyDescent="0.3">
-      <c r="J19" s="57"/>
+      <c r="J19" s="62"/>
       <c r="K19" s="1" t="s">
         <v>52</v>
       </c>
@@ -20747,7 +20823,7 @@
       <c r="Q19" s="6"/>
     </row>
     <row r="20" spans="10:24" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="J20" s="57"/>
+      <c r="J20" s="62"/>
       <c r="K20" s="1" t="s">
         <v>54</v>
       </c>
@@ -20768,7 +20844,7 @@
       </c>
     </row>
     <row r="21" spans="10:24" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="J21" s="57"/>
+      <c r="J21" s="62"/>
       <c r="K21" s="1" t="s">
         <v>59</v>
       </c>
@@ -20789,7 +20865,7 @@
       </c>
     </row>
     <row r="22" spans="10:24" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="J22" s="57"/>
+      <c r="J22" s="62"/>
       <c r="K22" s="1" t="s">
         <v>64</v>
       </c>
@@ -20813,7 +20889,7 @@
       </c>
     </row>
     <row r="23" spans="10:24" x14ac:dyDescent="0.3">
-      <c r="J23" s="57"/>
+      <c r="J23" s="62"/>
       <c r="K23" s="1" t="s">
         <v>68</v>
       </c>
@@ -20826,7 +20902,7 @@
       <c r="Q23" s="6"/>
     </row>
     <row r="24" spans="10:24" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="J24" s="57"/>
+      <c r="J24" s="62"/>
       <c r="K24" s="1" t="s">
         <v>70</v>
       </c>
@@ -20850,7 +20926,7 @@
       </c>
     </row>
     <row r="25" spans="10:24" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="J25" s="57"/>
+      <c r="J25" s="62"/>
       <c r="K25" s="1" t="s">
         <v>74</v>
       </c>
@@ -20874,7 +20950,7 @@
       </c>
     </row>
     <row r="26" spans="10:24" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="J26" s="57"/>
+      <c r="J26" s="62"/>
       <c r="K26" s="1" t="s">
         <v>79</v>
       </c>
@@ -20895,7 +20971,7 @@
       </c>
     </row>
     <row r="27" spans="10:24" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="J27" s="57"/>
+      <c r="J27" s="62"/>
       <c r="K27" s="10" t="s">
         <v>83</v>
       </c>
@@ -20922,21 +20998,21 @@
       <c r="X27" s="21"/>
     </row>
     <row r="28" spans="10:24" ht="14.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="J28" s="58" t="s">
+      <c r="J28" s="63" t="s">
         <v>87</v>
       </c>
-      <c r="K28" s="58"/>
+      <c r="K28" s="63"/>
       <c r="L28" s="19"/>
       <c r="M28" s="11"/>
-      <c r="O28" s="47" t="s">
+      <c r="O28" s="51" t="s">
         <v>87</v>
       </c>
-      <c r="P28" s="47"/>
-      <c r="Q28" s="47"/>
-      <c r="S28" s="47" t="s">
+      <c r="P28" s="51"/>
+      <c r="Q28" s="51"/>
+      <c r="S28" s="51" t="s">
         <v>87</v>
       </c>
-      <c r="T28" s="47"/>
+      <c r="T28" s="51"/>
     </row>
     <row r="29" spans="10:24" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
       <c r="K29" s="12" t="s">

</xml_diff>